<commit_message>
Unhide Answer in Excel file
</commit_message>
<xml_diff>
--- a/THE_WUR_MAC.xlsx
+++ b/THE_WUR_MAC.xlsx
@@ -3,18 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7BA302-9AF6-49A0-AC23-B8636027EBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFE6B122-A724-44C7-A51F-9F61E780F31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{15559836-0A5E-436A-BE14-4011178E8A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="2022 Global" sheetId="3" r:id="rId1"/>
-    <sheet name="2022 HKMO_Report_V(X)LOOKUP" sheetId="9" r:id="rId2"/>
-    <sheet name="2022HKMO_Report_V(X)LOOKUP_Done" sheetId="5" state="hidden" r:id="rId3"/>
-    <sheet name="18-22 MAC" sheetId="1" r:id="rId4"/>
-    <sheet name="18-22 MAC Report" sheetId="2" r:id="rId5"/>
-    <sheet name="18-22 MAC Report Formula" sheetId="7" r:id="rId6"/>
-    <sheet name="18-22 MAC Report Done " sheetId="8" state="hidden" r:id="rId7"/>
+    <sheet name="2022HKMO_Report_V(X)LOOKUP_Done" sheetId="5" r:id="rId2"/>
+    <sheet name="18-22 MAC" sheetId="1" r:id="rId3"/>
+    <sheet name="18-22 MAC Report Done " sheetId="8" r:id="rId4"/>
+    <sheet name="18-22 MAC Report Formula" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8529" uniqueCount="2301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8496" uniqueCount="2301">
   <si>
     <t>Rank</t>
   </si>
@@ -7008,7 +7006,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1" xr:uid="{BF2FD2F8-7AB6-4165-B34A-C93316AC1C46}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7027,7 +7025,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-TW"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7157,7 +7155,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7191,7 +7188,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7225,7 +7221,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7259,7 +7254,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7293,7 +7287,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7457,7 +7450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US" altLang="zh-TW"/>
+                    <a:endParaRPr lang="zh-TW" altLang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -7485,7 +7478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:endParaRPr lang="en-US" altLang="zh-TW"/>
+                    <a:endParaRPr lang="zh-TW" altLang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -7532,7 +7525,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7566,7 +7558,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7600,7 +7591,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -8494,7 +8484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -63745,97 +63735,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A37AE5B-F256-414C-9016-CF1B2B966F49}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2283</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2284</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>591</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7AD5A0-0798-4474-8E20-FB139EB61601}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -64150,7 +64049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BCC0EF-200E-4090-B5DF-AFAA95B26DB9}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -64437,12 +64336,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CB6783-E549-4EB2-BE60-50039F9C4F37}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA6FD10-9C43-4F9A-BAEF-A7E9432DBEDD}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.3"/>
@@ -64489,13 +64388,43 @@
       <c r="B2" t="s">
         <v>20</v>
       </c>
+      <c r="C2" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2293</v>
+      </c>
+      <c r="E2">
+        <v>-375.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2294</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2294</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2293</v>
+      </c>
+      <c r="E3">
+        <v>-375.5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2294</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2294</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -64505,8 +64434,26 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
+      <c r="C4" t="s">
+        <v>2295</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2296</v>
+      </c>
+      <c r="E4">
+        <v>-325.5</v>
+      </c>
       <c r="F4" t="s">
         <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2297</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2298</v>
+      </c>
+      <c r="I4">
+        <v>-275.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -64516,8 +64463,26 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
+      <c r="C5" t="s">
+        <v>2295</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2296</v>
+      </c>
+      <c r="E5">
+        <v>-325.5</v>
+      </c>
       <c r="F5" t="s">
         <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2297</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2298</v>
+      </c>
+      <c r="I5">
+        <v>-275.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -64527,23 +64492,42 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>2299</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2300</v>
+      </c>
+      <c r="E6">
+        <v>-225.5</v>
+      </c>
       <c r="F6" t="s">
         <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2297</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2298</v>
+      </c>
+      <c r="I6">
+        <v>-275.5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8194FB-7CA3-4AF0-A7DE-03E5F52861E3}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.3"/>
@@ -64757,190 +64741,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA6FD10-9C43-4F9A-BAEF-A7E9432DBEDD}">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="38.88671875" customWidth="1"/>
-    <col min="7" max="9" width="9.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2283</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2287</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2289</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2291</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2286</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2288</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2018</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2293</v>
-      </c>
-      <c r="E2">
-        <v>-375.5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2294</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2019</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2292</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2293</v>
-      </c>
-      <c r="E3">
-        <v>-375.5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2294</v>
-      </c>
-      <c r="H3" t="s">
-        <v>2294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2020</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2295</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2296</v>
-      </c>
-      <c r="E4">
-        <v>-325.5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2297</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2298</v>
-      </c>
-      <c r="I4">
-        <v>-275.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2021</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2295</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2296</v>
-      </c>
-      <c r="E5">
-        <v>-325.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2297</v>
-      </c>
-      <c r="H5" t="s">
-        <v>2298</v>
-      </c>
-      <c r="I5">
-        <v>-275.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2022</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2299</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2300</v>
-      </c>
-      <c r="E6">
-        <v>-225.5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2297</v>
-      </c>
-      <c r="H6" t="s">
-        <v>2298</v>
-      </c>
-      <c r="I6">
-        <v>-275.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>